<commit_message>
add: mor lpc and hpc pin and signal description, added links inside faq to appendix
</commit_message>
<xml_diff>
--- a/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
+++ b/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="High-pin count (HPC) connector" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Low-pin count (LPC) connector" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Pin and signal description" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="References" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="283">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -756,46 +757,178 @@
     <t xml:space="preserve">RES0</t>
   </si>
   <si>
-    <t xml:space="preserve">LA[00..33]_P, LA[00..33]_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User defined signals on Bank A located on the LPC and HPC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HA[00..23]_P, HA[00..23]_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User defined signals on Bank A located on the HPC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HB[00..21]_P, HB[00..21]_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User defined signals on Bank B located on the HPC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLK[0..3]_M2C_P, CLK[0..3]_M2C_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A differential pair that is assigned for a clock signal, which is driven from the carrier card to the IO Mezzanine Module.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBTCLK[0..1]_M2C_P, GBTCLK[0..1]_M2C_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP[0..9]_M2C_P, DP[0..9]_M2C_N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP[0..9]_C2M_P, DP[0..9]_C2M_N</t>
+    <t xml:space="preserve">LA[00..33]_P,
+LA[00..33]_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68 user-defined, single-ended signals or 34 user-defined, differential pairs (mandatory for LPC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HA[00..23]_P,
+HA[00..23]_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48 user-defined, single-ended signals or 24 user-defined, differential pairs (only HPC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HB[00..21]_P,
+HB[00..21]_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44 user-defined, single-ended signals or 22 user-defined, differential pairs (only HPC, 160 single ended / 80 differential signals in total)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLK[0..3]_M2C_P,
+CLK[0..3]_M2C_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 user clock, differential pairs (CLK[3..4]_M2C only for HPC), bidrectional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBTCLK[0..1]_M2C_P,
+GBTCLK[0..1]_M2C_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock signals for multi-gigabit transceiver data pairs (GBTCLK1_x only for HPC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP[0..9]_M2C_P,
+DP[0..9]_M2C_N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi-gigabit transceiver data pairs (one is mandatory for LPC, 10 in total with HPC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP[0..9]_C2M_P,
+DP[0..9]_C2M_N</t>
   </si>
   <si>
     <t xml:space="preserve">GA[0..1]</t>
   </si>
   <si>
-    <t xml:space="preserve">These signals provide geographical addressed of the module and are used for I2C channel select.</t>
+    <t xml:space="preserve">Geographical address of the module (can be used for adressing on I2C bus).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference voltage for signaling standard of bank A (LAxx and Haxx). Can be left floating, if not required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference voltage for signaling standard of bank A (Hbxx). Can be left floating, if not required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This voltage s sourced by the mezzanine module which supports the HB bus. It is used to power the IO Bank of the FPGA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3 V auxiliary power supply (max. 20 mA, max. 150 uF cap. Load).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustable voltage level (0 .. 3.3 V) from the carrier to the mezzanine card (max. 4 A, max. 1000 uF cap. load).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3 V power from the carrier to the mezzanine card (max. 3 A, max. 1000 uF cap. Load).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 V power from the carrier to the mezzanine card (max. 1 A, max. 1000 uF cap. Load).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG Reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG Mode Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG Data In, if JTAG chain is not used by mezzanine card, short TDI and TDO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG Data Out, if JTAG chain is not used by mezzanine card, short TDI and TDO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present signal. Indicates that a mezzanine module is attached to the carrier. Low active (tie to GND on FMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active high power good signal. High indicates that VADJ, 12P0V, and 3P3V are within tolerance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active high power good signal. High indicates that VIO_B_M2C, VREF_A_M2C, and VREF_B_M2C are within tolerance.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I2C serial clock. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Interface can support Intelligent Platform Management Interface (IPMI) commands.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">I2C serial data. Interface can support </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Intelligent Platform Management Interface (IPMI) commands.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">RES[0..1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved, left floating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANSI/VITA 57.1-2008</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Overview of VITA57 – FMC, Curtiss Wright, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">www.vita.com/Resources/Learn/FMC%20Overview.pptx</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">KC705 Evaluation Board for the Kintex-7 FPGA, Xilinx UG810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O Design Flexibility with the FPGA Mezzanine Card (FMC), Xilinx WP315</t>
   </si>
 </sst>
 </file>
@@ -805,11 +938,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -833,14 +967,32 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -873,14 +1025,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
         <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFF66"/>
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor rgb="FFCC99FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -955,7 +1113,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1012,7 +1170,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1064,7 +1282,7 @@
       <rgbColor rgb="FF99FF66"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF99FF"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF6666FF"/>
@@ -1095,17 +1313,17 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.12244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="15.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1138,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -1192,19 +1410,19 @@
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1227,19 +1445,19 @@
       <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1259,19 +1477,19 @@
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -1294,19 +1512,19 @@
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1320,264 +1538,264 @@
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>40</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="8" t="s">
         <v>48</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>52</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="8" t="s">
         <v>54</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>56</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>58</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>65</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>66</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>70</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>72</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>75</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>77</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="7" t="s">
+      <c r="J13" s="8" t="s">
         <v>78</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>84</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -1586,103 +1804,103 @@
       <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="8" t="s">
         <v>85</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>88</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>90</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>92</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>93</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>96</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>103</v>
       </c>
       <c r="H17" s="4" t="s">
@@ -1691,115 +1909,115 @@
       <c r="I17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="8" t="s">
         <v>104</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>106</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>107</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="8" t="s">
         <v>109</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>110</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>111</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>114</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="K19" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>121</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>122</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="8" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1807,31 +2025,31 @@
       <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>124</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>125</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>126</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="7" t="s">
         <v>127</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="9" t="s">
         <v>128</v>
       </c>
       <c r="K21" s="4" t="s">
@@ -1845,159 +2063,159 @@
       <c r="B22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>130</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>132</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="J22" s="9" t="s">
         <v>133</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>139</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>140</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K23" s="7" t="s">
+      <c r="K23" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>142</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>143</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="7" t="s">
         <v>144</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="H24" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>146</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>148</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>149</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="H25" s="7" t="s">
         <v>151</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="8" t="s">
         <v>152</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>158</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -2006,103 +2224,103 @@
       <c r="I26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="8" t="s">
         <v>159</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>160</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>161</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>162</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="8" t="s">
+      <c r="H27" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="7" t="s">
         <v>164</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K27" s="7" t="s">
+      <c r="K27" s="8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>166</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>167</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H28" s="8" t="s">
+      <c r="H28" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="7" t="s">
         <v>170</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="7" t="s">
+      <c r="K28" s="8" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="7" t="s">
         <v>177</v>
       </c>
       <c r="H29" s="4" t="s">
@@ -2111,182 +2329,182 @@
       <c r="I29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J29" s="7" t="s">
+      <c r="J29" s="8" t="s">
         <v>178</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>179</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>180</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>181</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H30" s="10" t="s">
         <v>182</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J30" s="7" t="s">
+      <c r="J30" s="8" t="s">
         <v>183</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>184</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>185</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H31" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="10" t="s">
         <v>188</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H32" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="10" t="s">
         <v>197</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K32" s="7" t="s">
+      <c r="K32" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>199</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>200</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>201</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="10" t="s">
         <v>202</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J33" s="7" t="s">
+      <c r="J33" s="8" t="s">
         <v>203</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>204</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>205</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="H34" s="9" t="s">
+      <c r="H34" s="10" t="s">
         <v>207</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J34" s="7" t="s">
+      <c r="J34" s="8" t="s">
         <v>208</v>
       </c>
       <c r="K34" s="4" t="s">
@@ -2297,34 +2515,34 @@
       <c r="A35" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="H35" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="10" t="s">
         <v>216</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="K35" s="8" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2332,34 +2550,34 @@
       <c r="A36" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>218</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>219</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="7" t="s">
         <v>220</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H36" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="I36" s="11" t="s">
         <v>222</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K36" s="7" t="s">
+      <c r="K36" s="8" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2370,92 +2588,92 @@
       <c r="B37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>224</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>225</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="12" t="s">
         <v>227</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J37" s="7" t="s">
+      <c r="J37" s="8" t="s">
         <v>228</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="7" t="s">
         <v>234</v>
       </c>
       <c r="H38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="J38" s="7" t="s">
+      <c r="J38" s="8" t="s">
         <v>235</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>236</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>237</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="7" t="s">
         <v>238</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="12" t="s">
         <v>227</v>
       </c>
       <c r="I39" s="4" t="s">
@@ -2464,7 +2682,7 @@
       <c r="J39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K39" s="7" t="s">
+      <c r="K39" s="8" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2481,25 +2699,25 @@
       <c r="D40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>241</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G40" s="13" t="s">
         <v>241</v>
       </c>
       <c r="H40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="11" t="s">
+      <c r="I40" s="12" t="s">
         <v>227</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="K40" s="8" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2513,19 +2731,19 @@
       <c r="C41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="13" t="s">
         <v>241</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="13" t="s">
         <v>241</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="H41" s="12" t="s">
         <v>227</v>
       </c>
       <c r="I41" s="4" t="s">
@@ -2556,17 +2774,17 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.12244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="15.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="15.1173469387755"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2599,930 +2817,930 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
       <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
       <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="7" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="7" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="9" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="8" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="8" t="s">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="8" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="7" t="s">
         <v>58</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="8" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="8" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="8" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="8" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="7" t="s">
         <v>77</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="8" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="8" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="7" t="s">
         <v>87</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="8" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="8" t="s">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="8" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="8" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="7" t="s">
         <v>106</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="8" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="7" t="s">
         <v>108</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="8" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="8" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
       <c r="H20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="8" t="s">
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="7" t="s">
         <v>125</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="8" t="s">
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="7" t="s">
         <v>127</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="8" t="s">
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="7" t="s">
         <v>132</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="8" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
       <c r="H23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="8" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="7" t="s">
         <v>143</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="8" t="s">
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="8" t="s">
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="7" t="s">
         <v>151</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="8" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
       <c r="H26" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="8" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="7" t="s">
         <v>161</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="8" t="s">
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="8" t="s">
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="8" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
       <c r="H29" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="8" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="7" t="s">
         <v>180</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="9" t="s">
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="10" t="s">
         <v>182</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="9" t="s">
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="8" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="9" t="s">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="8" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="7" t="s">
         <v>200</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="9" t="s">
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="10" t="s">
         <v>202</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="9" t="s">
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="10" t="s">
         <v>207</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="8" t="s">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="9" t="s">
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="8" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="7" t="s">
         <v>219</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="9" t="s">
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="I36" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="J36" s="13"/>
-      <c r="K36" s="13"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="11" t="s">
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="12" t="s">
         <v>227</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="8" t="s">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E38" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
       <c r="H38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="8" t="s">
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="7" t="s">
         <v>237</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="11" t="s">
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="12" t="s">
         <v>227</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
       <c r="H40" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="11" t="s">
+      <c r="I40" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="J40" s="13"/>
-      <c r="K40" s="13"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="12" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="13" t="s">
         <v>241</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="11" t="s">
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="12" t="s">
         <v>227</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
@@ -3535,176 +3753,353 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="3.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="107.928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="43.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="210.045918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="11.3418367346939"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="17" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="15" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="B9" s="15" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+    <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="B11" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="B13" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="B17" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="B19" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="B21" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="B23" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="24" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="B25" s="15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="26" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="B29" s="15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="22" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="B31" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="22" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="B33" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="22" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="B35" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="22" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="B37" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="22" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="B39" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="B41" s="15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="B43" s="15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="B45" s="15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="22" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="B47" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="22" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
+      <c r="B49" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="127.775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.530612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="www.vita.com/Resources/Learn/FMC%20Overview.pptx"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add: some info about GA pins add: description for _CC pins
</commit_message>
<xml_diff>
--- a/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
+++ b/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="High-pin count (HPC) connector" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="285">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -778,6 +778,13 @@
     <t xml:space="preserve">44 user-defined, single-ended signals or 22 user-defined, differential pairs (only HPC, 160 single ended / 80 differential signals in total)</t>
   </si>
   <si>
+    <t xml:space="preserve">XX_P_CC,
+XX_N_CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User-defined clock capable pins. These pins can be used for clock signals.</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLK[0..3]_M2C_P,
 CLK[0..3]_M2C_N</t>
   </si>
@@ -806,7 +813,7 @@
     <t xml:space="preserve">GA[0..1]</t>
   </si>
   <si>
-    <t xml:space="preserve">Geographical address of the module (can be used for adressing on I2C bus).</t>
+    <t xml:space="preserve">Geographical address of the module (can be used for adressing on I2C bus). These pins are driven by the carrier card.</t>
   </si>
   <si>
     <t xml:space="preserve">Reference voltage for signaling standard of bank A (LAxx and Haxx). Can be left floating, if not required.</t>
@@ -854,42 +861,10 @@
     <t xml:space="preserve">Active high power good signal. High indicates that VIO_B_M2C, VREF_A_M2C, and VREF_B_M2C are within tolerance.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">I2C serial clock. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Interface can support Intelligent Platform Management Interface (IPMI) commands.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">I2C serial data. Interface can support </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Intelligent Platform Management Interface (IPMI) commands.</t>
-    </r>
+    <t xml:space="preserve">I2C serial clock. Interface can support Intelligent Platform Management Interface (IPMI) commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C serial data. Interface can support Intelligent Platform Management Interface (IPMI) commands.</t>
   </si>
   <si>
     <t xml:space="preserve">RES[0..1]</t>
@@ -904,25 +879,7 @@
     <t xml:space="preserve">ANSI/VITA 57.1-2008</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Overview of VITA57 – FMC, Curtiss Wright, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">www.vita.com/Resources/Learn/FMC%20Overview.pptx</t>
-    </r>
+    <t xml:space="preserve">Overview of VITA57 – FMC, Curtiss Wright, www.vita.com/Resources/Learn/FMC%20Overview.pptx</t>
   </si>
   <si>
     <t xml:space="preserve">KC705 Evaluation Board for the Kintex-7 FPGA, Xilinx UG810</t>
@@ -974,15 +931,15 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1113,7 +1070,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1186,6 +1143,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1198,7 +1159,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1231,6 +1192,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1319,8 +1284,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2780,8 +2745,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3753,17 +3718,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B65536"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="3.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="43.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="210.045918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="207.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3774,6 +3739,10 @@
         <v>245</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+    </row>
     <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>246</v>
@@ -3782,6 +3751,10 @@
         <v>247</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+    </row>
     <row r="5" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
         <v>248</v>
@@ -3790,6 +3763,11 @@
         <v>249</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+    </row>
     <row r="7" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
         <v>250</v>
@@ -3798,6 +3776,10 @@
         <v>251</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="B8" s="0"/>
+    </row>
     <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="19" t="s">
         <v>252</v>
@@ -3806,6 +3788,10 @@
         <v>253</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+    </row>
     <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="20" t="s">
         <v>254</v>
@@ -3814,175 +3800,270 @@
         <v>255</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="0"/>
+    </row>
     <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
         <v>256</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>258</v>
-      </c>
+    </row>
+    <row r="16" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23" t="s">
+      <c r="B19" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="23" t="s">
+      <c r="B21" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="24" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="s">
+      <c r="B23" s="15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24" t="s">
-        <v>241</v>
-      </c>
       <c r="B25" s="15" t="s">
-        <v>263</v>
-      </c>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="25" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>264</v>
-      </c>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="B29" s="15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="s">
+      <c r="B31" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22" t="s">
+      <c r="B33" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="s">
+      <c r="B35" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+      <c r="B37" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="s">
-        <v>196</v>
-      </c>
       <c r="B39" s="15" t="s">
-        <v>270</v>
-      </c>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="23" t="s">
+      <c r="B43" s="15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="23" t="s">
+      <c r="B45" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+      <c r="B46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="22" t="s">
+      <c r="B47" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0"/>
+      <c r="B48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="22" t="s">
+      <c r="B49" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="23" t="s">
         <v>197</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27" t="s">
-        <v>276</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>277</v>
       </c>
     </row>
+    <row r="52" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0"/>
+      <c r="B52" s="0"/>
+    </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
-        <v>11</v>
+        <v>278</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0"/>
+      <c r="B54" s="0"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4001,15 +4082,15 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="127.775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="126.352040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4017,68 +4098,68 @@
         <v>1</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+        <v>281</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="B2" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="n">
         <v>3</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
+        <v>283</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="n">
         <v>4</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
+        <v>284</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4092,7 +4173,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="www.vita.com/Resources/Learn/FMC%20Overview.pptx"/>
+    <hyperlink ref="B2" r:id="rId1" display="Overview of VITA57 – FMC, Curtiss Wright, www.vita.com/Resources/Learn/FMC%20Overview.pptx"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
edit: fix bank to B (VREF_B_M2C pin)
</commit_message>
<xml_diff>
--- a/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
+++ b/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
@@ -816,10 +816,10 @@
     <t xml:space="preserve">Geographical address of the module (can be used for adressing on I2C bus). These pins are driven by the carrier card.</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference voltage for signaling standard of bank A (LAxx and Haxx). Can be left floating, if not required.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference voltage for signaling standard of bank A (Hbxx). Can be left floating, if not required.</t>
+    <t xml:space="preserve">Reference voltage for signaling standard of bank A (LAxx and Hbxx). Can be left floating, if not required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference voltage for signaling standard of bank B (Hbxx). Can be left floating, if not required.</t>
   </si>
   <si>
     <t xml:space="preserve">This voltage s sourced by the mezzanine module which supports the HB bus. It is used to power the IO Bank of the FPGA.</t>
@@ -895,7 +895,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -928,11 +928,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1070,7 +1065,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1143,10 +1138,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1159,7 +1150,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1195,7 +1186,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1284,8 +1275,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,8 +2736,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3720,15 +3711,15 @@
   </sheetPr>
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="3.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="207.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="205.459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3738,10 +3729,12 @@
       <c r="B1" s="17" t="s">
         <v>245</v>
       </c>
+      <c r="C1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
@@ -3750,10 +3743,12 @@
       <c r="B3" s="15" t="s">
         <v>247</v>
       </c>
+      <c r="C3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
@@ -3762,6 +3757,7 @@
       <c r="B5" s="15" t="s">
         <v>249</v>
       </c>
+      <c r="C5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
@@ -3769,7 +3765,7 @@
       <c r="C6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>250</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -3781,7 +3777,7 @@
       <c r="B8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>252</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -3793,7 +3789,7 @@
       <c r="B10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>254</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -3805,7 +3801,7 @@
       <c r="B12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>256</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -3817,7 +3813,7 @@
       <c r="B14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>258</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -3829,7 +3825,7 @@
       <c r="B16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>259</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -3841,7 +3837,7 @@
       <c r="B18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -3853,7 +3849,7 @@
       <c r="B20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="15" t="s">
@@ -3865,7 +3861,7 @@
       <c r="B22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="23" t="s">
         <v>240</v>
       </c>
       <c r="B23" s="15" t="s">
@@ -3877,7 +3873,7 @@
       <c r="B24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="22" t="s">
         <v>202</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -3889,7 +3885,7 @@
       <c r="B26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="24" t="s">
         <v>241</v>
       </c>
       <c r="B27" s="15" t="s">
@@ -3901,7 +3897,7 @@
       <c r="B28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="25" t="s">
         <v>227</v>
       </c>
       <c r="B29" s="15" t="s">
@@ -3913,7 +3909,7 @@
       <c r="B30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>222</v>
       </c>
       <c r="B31" s="15" t="s">
@@ -3925,7 +3921,7 @@
       <c r="B32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="22" t="s">
         <v>215</v>
       </c>
       <c r="B33" s="15" t="s">
@@ -3937,7 +3933,7 @@
       <c r="B34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="22" t="s">
         <v>182</v>
       </c>
       <c r="B35" s="15" t="s">
@@ -3949,7 +3945,7 @@
       <c r="B36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="22" t="s">
         <v>207</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -3961,7 +3957,7 @@
       <c r="B38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="22" t="s">
         <v>187</v>
       </c>
       <c r="B39" s="15" t="s">
@@ -3973,7 +3969,7 @@
       <c r="B40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="22" t="s">
         <v>196</v>
       </c>
       <c r="B41" s="15" t="s">
@@ -3985,7 +3981,7 @@
       <c r="B42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B43" s="15" t="s">
@@ -3997,7 +3993,7 @@
       <c r="B44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="23" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="15" t="s">
@@ -4009,7 +4005,7 @@
       <c r="B46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B47" s="15" t="s">
@@ -4021,7 +4017,7 @@
       <c r="B48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="22" t="s">
         <v>188</v>
       </c>
       <c r="B49" s="15" t="s">
@@ -4033,7 +4029,7 @@
       <c r="B50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="22" t="s">
         <v>197</v>
       </c>
       <c r="B51" s="15" t="s">
@@ -4045,7 +4041,7 @@
       <c r="B52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="27" t="s">
         <v>278</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -4057,7 +4053,7 @@
       <c r="B54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="15" t="s">
@@ -4089,8 +4085,8 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="126.352040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="124.867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,32 +4096,32 @@
       <c r="B1" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="n">
@@ -4134,15 +4130,15 @@
       <c r="B3" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="n">
@@ -4151,15 +4147,15 @@
       <c r="B4" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
edit: fix color of HPC pin J17 (GND)
</commit_message>
<xml_diff>
--- a/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
+++ b/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="High-pin count (HPC) connector" sheetId="1" state="visible" r:id="rId2"/>
@@ -1269,14 +1269,14 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,14 +1872,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="7" t="s">
@@ -2731,13 +2731,13 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="1" sqref="C18 H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.3112244897959"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3711,15 +3711,15 @@
   </sheetPr>
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="1" sqref="C18 B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="3.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="205.459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="203.163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4079,14 +4079,14 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C18 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="124.867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="123.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
edit: copyright year to 2018 add: pin summaries of HPC and LPC connectors fix: arrow marking pins in LPC image
</commit_message>
<xml_diff>
--- a/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
+++ b/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Low-pin count (LPC) connector" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Pin and signal description" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="References" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Summary" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="299">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -886,6 +887,48 @@
   </si>
   <si>
     <t xml:space="preserve">I/O Design Flexibility with the FPGA Mezzanine Card (FMC), Xilinx WP315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPC connector pin summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General pin function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gigabit data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gigabit clocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User clocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPC connector pin summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved</t>
   </si>
 </sst>
 </file>
@@ -895,7 +938,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -939,6 +982,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1024,7 +1074,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1037,6 +1087,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -1065,7 +1122,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1190,6 +1247,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1269,14 +1338,14 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.0408163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1347,7 +1416,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -1382,7 +1451,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
@@ -1417,7 +1486,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
@@ -1452,7 +1521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
@@ -1487,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
@@ -1872,7 +1941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
@@ -1977,7 +2046,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
@@ -2012,7 +2081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>21</v>
       </c>
@@ -2467,7 +2536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>34</v>
       </c>
@@ -2502,7 +2571,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>35</v>
       </c>
@@ -2537,7 +2606,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>36</v>
       </c>
@@ -2642,7 +2711,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>39</v>
       </c>
@@ -2677,7 +2746,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>40</v>
       </c>
@@ -2730,14 +2799,14 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="1" sqref="C18 H17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="14.0408163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2842,7 +2911,7 @@
       <c r="J4" s="14"/>
       <c r="K4" s="14"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
@@ -2865,7 +2934,7 @@
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
@@ -3118,7 +3187,7 @@
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
@@ -3709,62 +3778,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="1" sqref="C18 B23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="3.7"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="203.163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="200.867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="15" width="10.530612244898"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
         <v>244</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="C1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
         <v>246</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
       <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
         <v>248</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="C5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="3.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0"/>
       <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
         <v>250</v>
       </c>
@@ -3772,11 +3835,11 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0"/>
       <c r="B8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
         <v>252</v>
       </c>
@@ -3784,11 +3847,11 @@
         <v>253</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0"/>
       <c r="B10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
         <v>254</v>
       </c>
@@ -3796,11 +3859,11 @@
         <v>255</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="20" t="s">
         <v>256</v>
       </c>
@@ -3808,11 +3871,11 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
         <v>258</v>
       </c>
@@ -3820,7 +3883,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="0"/>
     </row>
@@ -3832,7 +3895,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0"/>
       <c r="B18" s="0"/>
     </row>
@@ -3844,7 +3907,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0"/>
       <c r="B20" s="0"/>
     </row>
@@ -3856,7 +3919,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="0"/>
     </row>
@@ -3868,7 +3931,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0"/>
     </row>
@@ -3880,7 +3943,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
       <c r="B26" s="0"/>
     </row>
@@ -3892,7 +3955,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0"/>
     </row>
@@ -3904,7 +3967,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="0"/>
     </row>
@@ -3916,7 +3979,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
       <c r="B32" s="0"/>
     </row>
@@ -3928,7 +3991,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
       <c r="B34" s="0"/>
     </row>
@@ -3940,7 +4003,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0"/>
     </row>
@@ -3952,7 +4015,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
       <c r="B38" s="0"/>
     </row>
@@ -3964,7 +4027,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0"/>
       <c r="B40" s="0"/>
     </row>
@@ -3976,7 +4039,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0"/>
       <c r="B42" s="0"/>
     </row>
@@ -3988,7 +4051,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0"/>
       <c r="B44" s="0"/>
     </row>
@@ -4000,7 +4063,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0"/>
       <c r="B46" s="0"/>
     </row>
@@ -4012,11 +4075,11 @@
         <v>275</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0"/>
       <c r="B48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="22" t="s">
         <v>188</v>
       </c>
@@ -4024,11 +4087,11 @@
         <v>276</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
       <c r="B50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="22" t="s">
         <v>197</v>
       </c>
@@ -4036,7 +4099,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0"/>
       <c r="B52" s="0"/>
     </row>
@@ -4048,7 +4111,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="3.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0"/>
       <c r="B54" s="0"/>
     </row>
@@ -4076,17 +4139,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C18 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="123.515306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="122.168367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4106,7 +4168,7 @@
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
     </row>
-    <row r="2" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="n">
         <v>2</v>
       </c>
@@ -4157,16 +4219,6 @@
       <c r="J4" s="29"/>
       <c r="K4" s="29"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Overview of VITA57 – FMC, Curtiss Wright, www.vita.com/Resources/Learn/FMC%20Overview.pptx"/>
@@ -4179,4 +4231,221 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.530612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" s="15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="15" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B11" s="15" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="31"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" s="15" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" s="15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" s="15" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B18" s="15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" s="15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B21" s="15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B22" s="15" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B23" s="15" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" s="15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A13:B13"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update pin descriptions according to website
</commit_message>
<xml_diff>
--- a/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
+++ b/appendix/VITA57_FMC_HPC_LPC_SIGNALS_AND_PINOUT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Desktop\FMCHUB\FMCHUB.github.io\appendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC0DD9B-2810-4072-AF5E-66ADCE9AFA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD78AE1-3A09-4083-82E0-F2AE6B45826E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="987" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="987" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-pin count (HPC) connector" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="302">
   <si>
     <t>K</t>
   </si>
@@ -776,13 +776,6 @@
     <t>User-defined clock capable pins. These pins can be used for clock signals.</t>
   </si>
   <si>
-    <t>CLK[0..3]_M2C_P,
-CLK[0..3]_M2C_N</t>
-  </si>
-  <si>
-    <t>4 user clock, differential pairs (CLK[3..4]_M2C only for HPC), bidrectional</t>
-  </si>
-  <si>
     <t>GBTCLK[0..1]_M2C_P,
 GBTCLK[0..1]_M2C_N</t>
   </si>
@@ -934,6 +927,23 @@
   </si>
   <si>
     <t>CLK2_BIDIR_N</t>
+  </si>
+  <si>
+    <t>2 user clocks, differential pairs, driver is the mezzanine module</t>
+  </si>
+  <si>
+    <t>2 user clocks, differential pairs, bidirectional (driver is determined by CLK_DIR pin)</t>
+  </si>
+  <si>
+    <t>CLK[2..3]_BIDIR_P,
+CLK[2..3]_BIDIR_N</t>
+  </si>
+  <si>
+    <t>CLK[0..1]_M2C_P,
+CLK[0..1]_M2C_N</t>
+  </si>
+  <si>
+    <t>Determines the driver for CLK[2..3]_BIDIR. GND (or floating) if the mezzanine module is the driver. 3P3V via 10k pull-up resistor if the carrier card drives the clock signals. Connection is made on the mezzanine module.</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1149,6 +1159,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1534,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -1606,7 +1625,7 @@
         <v>11</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>11</v>
@@ -1620,7 +1639,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>15</v>
@@ -1655,7 +1674,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>11</v>
@@ -1687,7 +1706,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
@@ -1722,7 +1741,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
@@ -3964,14 +3983,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK55"/>
+  <dimension ref="A1:AMK60"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.85546875" style="16"/>
-    <col min="2" max="2" width="200.85546875" style="16"/>
+    <col min="2" max="2" width="221.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5703125" style="16"/>
   </cols>
   <sheetData>
@@ -4025,289 +4046,317 @@
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13"/>
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15"/>
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B16" s="16" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10"/>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17"/>
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B18" s="16" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12"/>
-      <c r="B12"/>
-    </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19"/>
+      <c r="B19"/>
+    </row>
+    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B20" s="16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21"/>
+      <c r="B21"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14"/>
-      <c r="B14"/>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
+      <c r="B22" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16"/>
-      <c r="B16"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23"/>
+      <c r="B23"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="B17" s="16" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25"/>
+      <c r="B25"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18"/>
-      <c r="B18"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="16" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+      <c r="B27"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20"/>
-      <c r="B20"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="16" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29"/>
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22"/>
-      <c r="B22"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="B23" s="16" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31"/>
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="B32" s="16" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24"/>
-      <c r="B24"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="16" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33"/>
+      <c r="B33"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" s="16" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="B26"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="B27" s="16" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35"/>
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28"/>
-      <c r="B28"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B29" s="16" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30"/>
-      <c r="B30"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="B31" s="16" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39"/>
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32"/>
-      <c r="B32"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="B33" s="16" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41"/>
+      <c r="B41"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34"/>
-      <c r="B34"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" s="16" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43"/>
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B44" s="16" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36"/>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
-        <v>202</v>
-      </c>
-      <c r="B37" s="16" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45"/>
+      <c r="B45"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="16" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38"/>
-      <c r="B38"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B39" s="16" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47"/>
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40"/>
-      <c r="B40"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="B41" s="16" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49"/>
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="16" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42"/>
-      <c r="B42"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B43" s="16" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51"/>
+      <c r="B51"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="16" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44"/>
-      <c r="B44"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="16" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53"/>
+      <c r="B53"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46"/>
-      <c r="B46"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="16" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="B56" s="16" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48"/>
-      <c r="B48"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="B49" s="16" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="28" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50"/>
-      <c r="B50"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="B51" s="16" t="s">
+      <c r="B58" s="16" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52"/>
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="28" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54"/>
-      <c r="B54"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>275</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>
@@ -4334,7 +4383,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
@@ -4351,7 +4400,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -4368,7 +4417,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -4385,7 +4434,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -4423,21 +4472,21 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B3" s="16">
         <v>4</v>
@@ -4445,7 +4494,7 @@
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B4" s="16">
         <v>2</v>
@@ -4453,7 +4502,7 @@
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B5" s="16">
         <v>68</v>
@@ -4461,7 +4510,7 @@
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B6" s="16">
         <v>4</v>
@@ -4469,7 +4518,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B7" s="16">
         <v>2</v>
@@ -4477,7 +4526,7 @@
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B8" s="16">
         <v>5</v>
@@ -4485,7 +4534,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B9" s="16">
         <v>4</v>
@@ -4493,7 +4542,7 @@
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B10" s="16">
         <v>10</v>
@@ -4501,7 +4550,7 @@
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B11" s="16">
         <v>61</v>
@@ -4513,21 +4562,21 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B15" s="16">
         <v>40</v>
@@ -4535,7 +4584,7 @@
     </row>
     <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B16" s="16">
         <v>4</v>
@@ -4543,7 +4592,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B17" s="16">
         <v>160</v>
@@ -4551,7 +4600,7 @@
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B18" s="16">
         <v>8</v>
@@ -4559,7 +4608,7 @@
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B19" s="16">
         <v>2</v>
@@ -4567,7 +4616,7 @@
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B20" s="16">
         <v>5</v>
@@ -4575,7 +4624,7 @@
     </row>
     <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B21" s="16">
         <v>5</v>
@@ -4583,7 +4632,7 @@
     </row>
     <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B22" s="16">
         <v>15</v>
@@ -4591,7 +4640,7 @@
     </row>
     <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B23" s="16">
         <v>159</v>
@@ -4599,7 +4648,7 @@
     </row>
     <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B24" s="16">
         <v>2</v>

</xml_diff>